<commit_message>
Random Sleep 5-10 failed
</commit_message>
<xml_diff>
--- a/Multi_Glassdoor/glassdoor_job_data.xlsx
+++ b/Multi_Glassdoor/glassdoor_job_data.xlsx
@@ -547,12 +547,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>No Title Available</t>
+          <t>Sr. IT Recruiter</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Mesolith Software</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">

</xml_diff>

<commit_message>
Random Sleep 10-15 failed
</commit_message>
<xml_diff>
--- a/Multi_Glassdoor/glassdoor_job_data.xlsx
+++ b/Multi_Glassdoor/glassdoor_job_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,12 +473,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IT Executive</t>
+          <t>IT Helpdesk Analyst</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ametrine Nursing Care</t>
+          <t>Glitz Info Solutions</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -510,12 +510,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IT Helpdesk Analyst</t>
+          <t>Sr. IT Recruiter</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Glitz Info Solutions</t>
+          <t>Mesolith Software</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -547,12 +547,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sr. IT Recruiter</t>
+          <t>IT Support Specialist</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Mesolith Software</t>
+          <t>CyntraLabs TechLabs</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -621,12 +621,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>No Title Available</t>
+          <t>IT Intern</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Pixel Vision Technologies</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -658,12 +658,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>No Title Available</t>
+          <t>Solutions Architect</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>AbroadWorks Inc.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1612,6 +1612,1116 @@
         </is>
       </c>
       <c r="G32" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>No Title Available</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>No Title Available</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>No Title Available</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>No Title Available</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>No Title Available</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>No Title Available</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>No Title Available</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>No Title Available</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>No Title Available</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>No Title Available</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>No Title Available</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>No Title Available</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>No Title Available</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>No Title Available</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>No Title Available</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>No Title Available</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>IT Recruiter</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>WebPariwar</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>IT Executive</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Pinnacle Infotech</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>IT Systems Administrator</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Aastitva being foundation</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Executive IT</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Lotus Petal Charitable Foundation</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>IT - Information Technology</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Larsen &amp; Toubro</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>No Title Available</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>No Title Available</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>No Title Available</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>No Title Available</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>No Title Available</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>No Title Available</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>No Title Available</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>No Title Available</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>No Rating</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>No Title Available</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
         <is>
           <t>No Rating</t>
         </is>

</xml_diff>

<commit_message>
Random Sleep 10-25 failed
</commit_message>
<xml_diff>
--- a/Multi_Glassdoor/glassdoor_job_data.xlsx
+++ b/Multi_Glassdoor/glassdoor_job_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -584,12 +584,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>No Title Available</t>
+          <t>IT Intern</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Pixel Vision Technologies</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -621,12 +621,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>IT Intern</t>
+          <t>No Title Available</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Pixel Vision Technologies</t>
+          <t>No Company Name Available</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -658,12 +658,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Solutions Architect</t>
+          <t>Work from Home IT Counselors</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>AbroadWorks Inc.</t>
+          <t>Nestsoft technologies</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -695,12 +695,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>No Title Available</t>
+          <t>IT Recruiter</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>CYNOSURE TECHNOLOGIES PVT LTD</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -880,12 +880,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>No Title Available</t>
+          <t>IT Testing</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Infosys</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -954,12 +954,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>No Title Available</t>
+          <t>IT Executive</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Central Park</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -991,12 +991,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>No Title Available</t>
+          <t>IT Counselor (Work from Home) Hindi, Tamil, Malayalam</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Nestsoft technologies</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1250,12 +1250,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>No Title Available</t>
+          <t>IT Executive (Software)</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Nirali Hospital</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1361,12 +1361,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>No Title Available</t>
+          <t>MCA, BE, B.Tech, M.Tech &amp; IT Professional Required</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>BISP SOLUTIONS</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1546,12 +1546,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>No Title Available</t>
+          <t>Wanted IT Freshers (KeralaDaily.com)</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Nestsoft technologies</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1612,1116 +1612,6 @@
         </is>
       </c>
       <c r="G32" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>No Title Available</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>No Company Name Available</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>No Title Available</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>No Company Name Available</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>No Title Available</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>No Company Name Available</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>No Title Available</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>No Company Name Available</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>No Title Available</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>No Company Name Available</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>No Title Available</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>No Company Name Available</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>No Title Available</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>No Company Name Available</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>No Title Available</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>No Company Name Available</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>No Title Available</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>No Company Name Available</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>No Title Available</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>No Company Name Available</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>No Title Available</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>No Company Name Available</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>No Title Available</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>No Company Name Available</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>No Title Available</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>No Company Name Available</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>No Title Available</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>No Company Name Available</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>No Title Available</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>No Company Name Available</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>No Title Available</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>No Company Name Available</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>IT Recruiter</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>WebPariwar</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>IT Executive</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>Pinnacle Infotech</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>IT Systems Administrator</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>Aastitva being foundation</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>Executive IT</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>Lotus Petal Charitable Foundation</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>IT - Information Technology</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>Larsen &amp; Toubro</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>No Title Available</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>No Company Name Available</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>No Title Available</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>No Company Name Available</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>No Title Available</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>No Company Name Available</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>No Title Available</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>No Company Name Available</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>No Title Available</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>No Company Name Available</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>No Title Available</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>No Company Name Available</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>No Title Available</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>No Company Name Available</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>No Title Available</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>No Company Name Available</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>No Rating</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>No Title Available</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>No Company Name Available</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>No Location Available</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr">
         <is>
           <t>No Rating</t>
         </is>

</xml_diff>